<commit_message>
multifunction added; corrected global var to account for col count of all 3 tabs
</commit_message>
<xml_diff>
--- a/OutputFiles/TC01_Canine_Filter_Breed-Akita_WebData.xlsx
+++ b/OutputFiles/TC01_Canine_Filter_Breed-Akita_WebData.xlsx
@@ -12,9 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>Sample ID</t>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>File Type</t>
+  </si>
+  <si>
+    <t>Association</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Size</t>
   </si>
   <si>
     <t>Case ID</t>
@@ -26,31 +41,25 @@
     <t>Diagnosis</t>
   </si>
   <si>
-    <t>Sample Site</t>
+    <t>Study Code</t>
   </si>
   <si>
-    <t>Sample Type</t>
+    <t>CCB010072.pdf</t>
   </si>
   <si>
-    <t>Pathology/Morphology</t>
+    <t>Pathology Report</t>
   </si>
   <si>
-    <t>Tumor Grade</t>
+    <t>diagnosis</t>
   </si>
   <si>
-    <t>Sample Chronology</t>
+    <t/>
   </si>
   <si>
-    <t>Percentage Tumor</t>
+    <t>pdf</t>
   </si>
   <si>
-    <t>Necropsy Sample</t>
-  </si>
-  <si>
-    <t>Sample Preservation</t>
-  </si>
-  <si>
-    <t>NCATS-COP01-CCB010072 0103</t>
+    <t>57.73 KB</t>
   </si>
   <si>
     <t>NCATS-COP01-CCB010072</t>
@@ -62,37 +71,7 @@
     <t>Osteosarcoma</t>
   </si>
   <si>
-    <t>Humerus</t>
-  </si>
-  <si>
-    <t>Primary Malignant Tumor Tissue</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>Not Applicable</t>
-  </si>
-  <si>
-    <t>34.19</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Snap Frozen</t>
-  </si>
-  <si>
-    <t>NCATS-COP01-CCB010072 0311</t>
-  </si>
-  <si>
-    <t>Blood</t>
-  </si>
-  <si>
-    <t>Whole Blood</t>
-  </si>
-  <si>
-    <t/>
+    <t>NCATS-COP01</t>
   </si>
 </sst>
 </file>
@@ -137,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -174,87 +153,37 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>